<commit_message>
age, address and decode time
</commit_message>
<xml_diff>
--- a/backend/DataBase/shop_1030am.xlsx
+++ b/backend/DataBase/shop_1030am.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vasantha Raj\Desktop\FairPriceApp\backend\DataBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEA358D1-0D1E-435A-92FD-4071F1063C9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8987C4D0-3D70-4E83-996B-8C5B02F08BE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4FF77EA4-3A67-4EC4-8310-27D263F9955A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
   <si>
     <t>shop_id</t>
   </si>
@@ -127,6 +127,18 @@
   </si>
   <si>
     <t>efg@shop.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10:00:00 </t>
+  </si>
+  <si>
+    <t>10:00:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10:30:00 </t>
+  </si>
+  <si>
+    <t>10:30:00</t>
   </si>
 </sst>
 </file>
@@ -178,7 +190,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -497,11 +509,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1820624-63B2-4BD4-8915-6CB548E4E46B}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="19.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -538,7 +550,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>201</v>
       </c>
@@ -554,8 +566,8 @@
       <c r="E2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="3">
-        <v>0.41666666666666669</v>
+      <c r="F2" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>14</v>
@@ -563,8 +575,8 @@
       <c r="H2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="3">
-        <v>0.4375</v>
+      <c r="I2" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>16</v>
@@ -573,7 +585,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>202</v>
       </c>
@@ -589,8 +601,8 @@
       <c r="E3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="3">
-        <v>0.41666666666666669</v>
+      <c r="F3" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>21</v>
@@ -598,8 +610,8 @@
       <c r="H3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="3">
-        <v>0.4375</v>
+      <c r="I3" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>16</v>
@@ -608,7 +620,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>203</v>
       </c>
@@ -624,8 +636,8 @@
       <c r="E4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="3">
-        <v>0.41666666666666669</v>
+      <c r="F4" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>14</v>
@@ -633,8 +645,8 @@
       <c r="H4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I4" s="3">
-        <v>0.4375</v>
+      <c r="I4" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>16</v>
@@ -643,7 +655,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>204</v>
       </c>
@@ -659,8 +671,8 @@
       <c r="E5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="3">
-        <v>0.41666666666666669</v>
+      <c r="F5" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>14</v>
@@ -668,8 +680,8 @@
       <c r="H5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="I5" s="3">
-        <v>0.4375</v>
+      <c r="I5" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>16</v>
@@ -678,7 +690,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>205</v>
       </c>
@@ -694,8 +706,8 @@
       <c r="E6" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="3">
-        <v>0.41666666666666669</v>
+      <c r="F6" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>21</v>
@@ -703,8 +715,8 @@
       <c r="H6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="I6" s="3">
-        <v>0.4375</v>
+      <c r="I6" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>16</v>

</xml_diff>